<commit_message>
finalisation version appels de marge
</commit_message>
<xml_diff>
--- a/ex_future.xlsx
+++ b/ex_future.xlsx
@@ -1,31 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\data\Documents\Divers intéressant\Secteur financier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00276D10-9F75-49C4-A78A-148BA529504F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11460"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sans_appels_marge" sheetId="3" r:id="rId1"/>
     <sheet name="Avec_appels_marge" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>chris</author>
+  </authors>
+  <commentList>
+    <comment ref="L21" authorId="0" shapeId="0" xr:uid="{2FD62AF1-DDEA-42FA-9DE8-9956C426E6B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>chris:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Principes :
+- marge initiale = 10%
+- complétée de manière à couvrir en permanence le résultat du débouclement de l'opération + conserver la marge initiale</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="54">
   <si>
     <t>Opérations</t>
   </si>
@@ -138,9 +181,6 @@
     <t>Pour déboucler future, soit (prise de) livraison, soit transaction inverse</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Valeur prévue initialement par future - utilisation marge accumulée</t>
   </si>
   <si>
@@ -156,29 +196,67 @@
     <t>Solde vente t+3</t>
   </si>
   <si>
-    <t>Valeur prévue initialement par future + marge déjà versée</t>
-  </si>
-  <si>
     <t>Récupération marge versée</t>
   </si>
   <si>
-    <t>En fait, utilisé pour pmt future</t>
-  </si>
-  <si>
-    <t>En fait, utilisé pour achat spot</t>
+    <t>marge</t>
+  </si>
+  <si>
+    <t>Marge demandée t+2</t>
+  </si>
+  <si>
+    <t>Marge demandée t+3</t>
+  </si>
+  <si>
+    <t>Appel de marge t+2</t>
+  </si>
+  <si>
+    <t>Appel de marge t+3</t>
+  </si>
+  <si>
+    <t>Optique : broker</t>
+  </si>
+  <si>
+    <t>Récupération marge initiale</t>
+  </si>
+  <si>
+    <t>Appels de marge = étalement dans le temps de la différence finale à encaisser/verser</t>
+  </si>
+  <si>
+    <t>Somme a.m. achat</t>
+  </si>
+  <si>
+    <t>Somme a.m. vente</t>
+  </si>
+  <si>
+    <t>Pmt effectif hors récup. Marge</t>
+  </si>
+  <si>
+    <t>Pmt effectif hors récup. marge</t>
+  </si>
+  <si>
+    <t>dont appels de m. déjà reçus</t>
+  </si>
+  <si>
+    <t>Solde (à recevoir/payer)</t>
+  </si>
+  <si>
+    <t>Optique : client</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _C_H_F_-;\-* #,##0.00\ _C_H_F_-;_-* &quot;-&quot;??\ _C_H_F_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0\ _C_H_F_-;\-* #,##0.0\ _C_H_F_-;_-* &quot;-&quot;?\ _C_H_F_-;_-@_-"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _C_H_F_-;\-* #,##0.00\ _C_H_F_-;_-* &quot;-&quot;??\ _C_H_F_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.0\ _C_H_F_-;\-* #,##0.0\ _C_H_F_-;_-* &quot;-&quot;?\ _C_H_F_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;?_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +302,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -233,7 +336,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -241,38 +344,168 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -553,11 +786,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -574,32 +807,32 @@
     <col min="12" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
@@ -607,7 +840,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -626,8 +859,11 @@
       <c r="H10" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I10" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -654,12 +890,12 @@
         <f t="shared" si="0"/>
         <v>10612.079999999998</v>
       </c>
-      <c r="J11" s="4">
+      <c r="I11" s="4">
         <f>H11-G11</f>
         <v>208.07999999999811</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -687,7 +923,7 @@
         <v>12484.8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -715,7 +951,7 @@
         <v>11220</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -736,131 +972,136 @@
         <v>8000</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>10</v>
+      <c r="J17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>38</v>
+      <c r="A18" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>1</v>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="6">
+        <f>-0.1*G11</f>
+        <v>-1040.4000000000001</v>
+      </c>
+      <c r="J19" s="12">
+        <f>D19</f>
+        <v>-1040.4000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D20" s="6">
-        <f>-0.1*G12</f>
-        <v>-1224</v>
-      </c>
-      <c r="J20" s="13">
+        <f>-0.1*H11</f>
+        <v>-1061.2079999999999</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="11">
         <f>D20</f>
-        <v>-1224</v>
+        <v>-1061.2079999999999</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="6">
-        <f>-0.1*H12</f>
-        <v>-1248.48</v>
-      </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="12">
-        <f>D21</f>
-        <v>-1248.48</v>
-      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="J22" s="13"/>
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="J23" s="13"/>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="6">
+        <f>-F13</f>
+        <v>-11000</v>
+      </c>
+      <c r="J23" s="12">
+        <f>J19+D23</f>
+        <v>-12040.4</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="6">
-        <f>-F13</f>
-        <v>-11000</v>
-      </c>
-      <c r="J24" s="13">
-        <f>J20+D24</f>
-        <v>-12224</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="J25" s="13"/>
+      <c r="C25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="10">
+        <f>-G11</f>
+        <v>-10404</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="12"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D26" s="6">
-        <f>-G11</f>
-        <v>-10404</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" s="13">
-        <f>J24+D26</f>
-        <v>-22628</v>
+        <f>-D19</f>
+        <v>1040.4000000000001</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="J26" s="12">
+        <f>J23+D26</f>
+        <v>-11000</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="6">
-        <f>-D20</f>
-        <v>1224</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J27" s="13">
-        <f>J26+D27</f>
-        <v>-21404</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C28" s="1" t="s">
+      <c r="C27" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D27" s="10">
         <f>F13</f>
         <v>11000</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="14">
-        <f>J27+D28</f>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C28" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="28">
+        <f>D25+D27</f>
+        <v>596</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="J28" s="13">
+        <f>J26+D28</f>
         <v>-10404</v>
       </c>
     </row>
@@ -882,8 +1123,8 @@
         <v>8000</v>
       </c>
       <c r="K31" s="4">
-        <f>D31+K21</f>
-        <v>6751.52</v>
+        <f>D31+K20</f>
+        <v>6938.7920000000004</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -893,52 +1134,59 @@
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="10">
         <f>H11</f>
         <v>10612.079999999998</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K33" s="4">
-        <f>K31+D33</f>
-        <v>17363.599999999999</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="K33" s="4"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D34" s="6">
-        <f>-D21</f>
-        <v>1248.48</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>42</v>
-      </c>
+        <f>-D20</f>
+        <v>1061.2079999999999</v>
+      </c>
+      <c r="E34" s="5"/>
       <c r="K34" s="4">
-        <f>K33+D34</f>
-        <v>18612.079999999998</v>
+        <f>K31+D34</f>
+        <v>8000</v>
       </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="27">
         <f>-F14</f>
         <v>-8000</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K35" s="14">
-        <f>K34+D35</f>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C36" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="28">
+        <f>D33+D35</f>
+        <v>2612.0799999999981</v>
+      </c>
+      <c r="K36" s="13">
+        <f>K34+D36</f>
         <v>10612.079999999998</v>
       </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="J38" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -947,14 +1195,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A2:K43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:P58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -963,50 +1208,52 @@
     <col min="2" max="2" width="15.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="1"/>
+    <col min="5" max="5" width="14.125" style="1" customWidth="1"/>
     <col min="6" max="8" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="11" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="1"/>
+    <col min="12" max="13" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1025,8 +1272,11 @@
       <c r="H10" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I10" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1053,12 +1303,12 @@
         <f t="shared" ref="H11:H14" si="1">D11*100</f>
         <v>10612.079999999998</v>
       </c>
-      <c r="J11" s="4">
+      <c r="I11" s="16">
         <f>H11-G11</f>
         <v>208.07999999999811</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1086,7 +1336,7 @@
         <v>12484.8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1114,7 +1364,7 @@
         <v>11220</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1135,293 +1385,525 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B17" s="36"/>
+      <c r="C17" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="38">
+        <f>D29+D34</f>
+        <v>596</v>
+      </c>
+      <c r="E17" s="39">
+        <f>F13-D17</f>
+        <v>10404</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="42">
+        <f>D30+D35+D48</f>
+        <v>2612.0799999999972</v>
+      </c>
+      <c r="E18" s="43">
+        <f>D18+D49</f>
+        <v>10612.079999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J17" s="1" t="s">
+      <c r="J21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="L22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D24" s="6">
         <f>-0.1*G11</f>
         <v>-1040.4000000000001</v>
       </c>
-      <c r="J19" s="12">
-        <f>D19</f>
+      <c r="J24" s="11">
+        <f>D24</f>
         <v>-1040.4000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+      <c r="L24" s="11">
+        <f>-D24</f>
+        <v>1040.4000000000001</v>
+      </c>
+      <c r="M24" s="11">
+        <f>-D25</f>
+        <v>1061.2079999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D25" s="6">
         <f>-0.1*H11</f>
         <v>-1061.2079999999999</v>
       </c>
-      <c r="K20" s="12">
-        <f>D20</f>
+      <c r="K25" s="11">
+        <f>D25</f>
         <v>-1061.2079999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:16" s="17" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="6">
-        <f>G12-G11</f>
+      <c r="D29" s="24">
+        <f>-N29</f>
         <v>1836</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="15">
+        <f>J24+D29</f>
+        <v>795.59999999999991</v>
+      </c>
+      <c r="L29" s="21">
+        <f>G11-G12+$L$24</f>
+        <v>-795.59999999999991</v>
+      </c>
+      <c r="M29" s="20"/>
+      <c r="N29" s="19">
+        <f>L29-L24</f>
+        <v>-1836</v>
+      </c>
+      <c r="P29" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="24">
+        <f>-O30</f>
+        <v>-1872.7200000000018</v>
+      </c>
+      <c r="E30" s="24"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="K30" s="15">
+        <f>K25+D30</f>
+        <v>-2933.9280000000017</v>
+      </c>
+      <c r="M30" s="21">
+        <f>$M$24+H12-H11</f>
+        <v>2933.9280000000017</v>
+      </c>
+      <c r="O30" s="19">
+        <f>M30-M24</f>
+        <v>1872.7200000000018</v>
+      </c>
+      <c r="P30" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="4">
-        <f>J19+D24</f>
-        <v>795.59999999999991</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D31" s="6"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B34" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="6">
+        <f>-N34</f>
+        <v>-1240</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="25">
+        <f>J29+D34</f>
+        <v>-444.40000000000009</v>
+      </c>
+      <c r="L34" s="25">
+        <f>L24+(G11-G13)</f>
+        <v>444.40000000000009</v>
+      </c>
+      <c r="N34" s="25">
+        <f>L34-L29</f>
+        <v>1240</v>
+      </c>
+      <c r="P34" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="6">
-        <f>-(H12-H11)</f>
-        <v>-1872.7200000000012</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K25" s="4">
-        <f>K20+D25</f>
-        <v>-2933.9280000000008</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11">
-        <f>D24+D25</f>
-        <v>-36.720000000001164</v>
-      </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="6">
-        <f>-(H13-H12)</f>
+      <c r="D35" s="24">
+        <f>-O35</f>
         <v>1264.7999999999993</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="K35" s="15">
+        <f>K30+D35</f>
+        <v>-1669.1280000000024</v>
+      </c>
+      <c r="M35" s="21">
+        <f>$M$24+H13-H11</f>
+        <v>1669.1280000000024</v>
+      </c>
+      <c r="N35" s="21"/>
+      <c r="O35" s="19">
+        <f>M35-M30</f>
+        <v>-1264.7999999999993</v>
+      </c>
+      <c r="P35" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K30" s="4">
-        <f>K25+D30</f>
-        <v>-1669.1280000000015</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="3"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B36" s="3"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D37" s="6">
         <f>-F13</f>
         <v>-11000</v>
       </c>
-      <c r="J32" s="4">
-        <f>J24+D32</f>
-        <v>-10204.4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
+      <c r="J37" s="4">
+        <f>J34+D37</f>
+        <v>-11444.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C34" s="1" t="s">
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C39" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D39" s="10">
         <f>-G11</f>
         <v>-10404</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J34" s="4">
-        <f>J32+D34</f>
-        <v>-20608.400000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="6">
-        <f>-(D19+D24)</f>
-        <v>-795.59999999999991</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J35" s="4">
-        <f>J34+D35</f>
-        <v>-21404</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C36" s="1" t="s">
+      <c r="E39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="6">
+        <f>-D24</f>
+        <v>1040.4000000000001</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="J40" s="4">
+        <f>J37+D40</f>
+        <v>-10404</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C41" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D41" s="10">
         <f>F13</f>
         <v>11000</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J36" s="4">
-        <f>J35+D36</f>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C42" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="26">
+        <f>D39+D41</f>
+        <v>596</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="J42" s="13"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C43" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="31">
+        <f>D29+D34</f>
+        <v>596</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="J43" s="13"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C44" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="32">
+        <f>D42-D43</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="13">
+        <f>J40+D44</f>
         <v>-10404</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J45" s="13"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+    </row>
+    <row r="48" spans="1:16" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="24">
+        <f>-O48</f>
+        <v>3220</v>
+      </c>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="K48" s="15">
+        <f>K35+D48</f>
+        <v>1550.8719999999976</v>
+      </c>
+      <c r="M48" s="21">
+        <f>$M$24+H14-H11</f>
+        <v>-1550.8719999999976</v>
+      </c>
+      <c r="N48" s="21"/>
+      <c r="O48" s="19">
+        <f>M48-M35</f>
+        <v>-3220</v>
+      </c>
+      <c r="P48" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D49" s="6">
         <f>F14</f>
         <v>8000</v>
       </c>
-      <c r="K39" s="4">
-        <f>K30+D39</f>
-        <v>6330.8719999999985</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+      <c r="K49" s="4">
+        <f>K48+D49</f>
+        <v>9550.8719999999976</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="6"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C41" s="1" t="s">
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C51" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D51" s="10">
         <f>H11</f>
         <v>10612.079999999998</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E51" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K41" s="4">
-        <f>K39+D41</f>
-        <v>16942.951999999997</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="6">
-        <f>-D29</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K42" s="4">
-        <f>K41+D42</f>
-        <v>16942.951999999997</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C43" s="1" t="s">
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="6">
+        <f>-D25</f>
+        <v>1061.2079999999999</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="K52" s="4">
+        <f>K49+D52</f>
+        <v>10612.079999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C53" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D53" s="27">
         <f>-F14</f>
         <v>-8000</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K43" s="4">
-        <f>K42+D43</f>
-        <v>8942.9519999999975</v>
-      </c>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C54" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="26">
+        <f>D51+D53</f>
+        <v>2612.0799999999981</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C55" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" s="26">
+        <f>D30+D35+D48</f>
+        <v>2612.0799999999972</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C56" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="28">
+        <f>D54-D55</f>
+        <v>0</v>
+      </c>
+      <c r="K56" s="13">
+        <f>K52+D56</f>
+        <v>10612.079999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D57" s="25"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D58" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>